<commit_message>
Updated trapping nights to include treatments
</commit_message>
<xml_diff>
--- a/Data/Parkes Trapping Nights.xlsx
+++ b/Data/Parkes Trapping Nights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a29484792b23b3e/Documents/data/Mice/Mouse Ecology Proj/Parkes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="8_{ECBBB11F-3933-4177-AF68-3D8662404C3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{280711BE-DBA2-40AE-B2AE-E92F52243657}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="8_{ECBBB11F-3933-4177-AF68-3D8662404C3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{752222E0-F60C-42C2-9D31-C02A72322C33}"/>
   <bookViews>
-    <workbookView xWindow="31690" yWindow="-1670" windowWidth="17280" windowHeight="13630" xr2:uid="{796BBAF7-74DC-4E16-9375-B9ACD4BB880D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{796BBAF7-74DC-4E16-9375-B9ACD4BB880D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="26">
   <si>
     <t>DataSiteName</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>AnField 2</t>
+  </si>
+  <si>
+    <t>preharvest</t>
+  </si>
+  <si>
+    <t>postharvest</t>
+  </si>
+  <si>
+    <t>pre-rolling</t>
+  </si>
+  <si>
+    <t>post-rolling</t>
+  </si>
+  <si>
+    <t>Manipulation</t>
   </si>
 </sst>
 </file>
@@ -451,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE996D2C-4228-4399-BB0D-30FC198B9E24}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,9 +477,10 @@
     <col min="1" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -483,8 +499,11 @@
       <c r="F1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -503,8 +522,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -523,8 +545,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -543,8 +568,11 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -563,8 +591,11 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -583,8 +614,11 @@
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -603,8 +637,11 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -623,8 +660,11 @@
       <c r="F8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -643,8 +683,11 @@
       <c r="F9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -663,8 +706,11 @@
       <c r="F10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -683,8 +729,11 @@
       <c r="F11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -703,8 +752,11 @@
       <c r="F12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -723,8 +775,11 @@
       <c r="F13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -743,8 +798,11 @@
       <c r="F14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -763,8 +821,11 @@
       <c r="F15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -783,8 +844,11 @@
       <c r="F16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -803,8 +867,11 @@
       <c r="F17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -823,8 +890,11 @@
       <c r="F18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -843,8 +913,11 @@
       <c r="F19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -863,8 +936,11 @@
       <c r="F20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -883,8 +959,11 @@
       <c r="F21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -903,8 +982,11 @@
       <c r="F22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -923,8 +1005,11 @@
       <c r="F23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -943,8 +1028,11 @@
       <c r="F24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -963,8 +1051,11 @@
       <c r="F25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -983,8 +1074,11 @@
       <c r="F26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1003,8 +1097,11 @@
       <c r="F27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1023,8 +1120,11 @@
       <c r="F28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1043,8 +1143,11 @@
       <c r="F29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1063,8 +1166,11 @@
       <c r="F30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1082,6 +1188,9 @@
       </c>
       <c r="F31">
         <v>5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>